<commit_message>
Sistema de Dialogos Creado
</commit_message>
<xml_diff>
--- a/Assets/Dialogues/DialogosDUM.xlsx
+++ b/Assets/Dialogues/DialogosDUM.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Dialogo</t>
   </si>
@@ -112,12 +109,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,28 +142,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>